<commit_message>
update bai tap assignment hoan chinh
</commit_message>
<xml_diff>
--- a/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/dat-hang-thanh-toan.xlsx
+++ b/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/dat-hang-thanh-toan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -113,16 +113,19 @@
     <t>Trần Thị Hằng</t>
   </si>
   <si>
-    <t>hahaaaa17@gmail.com</t>
-  </si>
-  <si>
-    <t>hanghang@gmail.com</t>
-  </si>
-  <si>
-    <t>hahaaaa19@gmail.com</t>
-  </si>
-  <si>
-    <t>hahaaa164@gmail.com</t>
+    <t>hahaaa25@gmail.com</t>
+  </si>
+  <si>
+    <t>hahaaaa26@gmail.com</t>
+  </si>
+  <si>
+    <t>hahaaa3334@gmail.com</t>
+  </si>
+  <si>
+    <t>Hang12345@</t>
+  </si>
+  <si>
+    <t>tran22@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +547,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -606,7 +609,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -663,15 +666,33 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>1234</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4">
+        <v>553366566</v>
+      </c>
+      <c r="R4">
+        <v>23567777</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
+      <c r="T4">
+        <v>2026</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -679,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -726,8 +747,8 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chay lai file test suite
</commit_message>
<xml_diff>
--- a/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/dat-hang-thanh-toan.xlsx
+++ b/assignment/tran-thi-hang/assigment-webui/Data Files/excel-data/dat-hang-thanh-toan.xlsx
@@ -113,19 +113,19 @@
     <t>Trần Thị Hằng</t>
   </si>
   <si>
-    <t>hahaaa25@gmail.com</t>
-  </si>
-  <si>
-    <t>hahaaaa26@gmail.com</t>
-  </si>
-  <si>
-    <t>hahaaa3334@gmail.com</t>
-  </si>
-  <si>
     <t>Hang12345@</t>
   </si>
   <si>
     <t>tran22@gmail.com</t>
+  </si>
+  <si>
+    <t>hahaaaa27@gmail.com</t>
+  </si>
+  <si>
+    <t>hahaaa44@gmail.com</t>
+  </si>
+  <si>
+    <t>hahaaa5555@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +547,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -609,7 +609,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -671,10 +671,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>27</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>

</xml_diff>